<commit_message>
fix test case 5
</commit_message>
<xml_diff>
--- a/at_amazon/src/test/resources/data/data_order.xlsx
+++ b/at_amazon/src/test/resources/data/data_order.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>ID TC</t>
   </si>
@@ -48,9 +48,6 @@
     <t>0879231543</t>
   </si>
   <si>
-    <t>11616</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>Please provide a valid phone number</t>
   </si>
   <si>
-    <t>We couldn't verify your address. Please make sure it's correct before you save it.</t>
-  </si>
-  <si>
     <t>abc</t>
   </si>
   <si>
@@ -96,7 +90,7 @@
     <t>05</t>
   </si>
   <si>
-    <t>06</t>
+    <t>100000</t>
   </si>
 </sst>
 </file>
@@ -461,7 +455,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -469,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,18 +498,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -524,41 +518,41 @@
         <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -570,18 +564,18 @@
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -593,18 +587,18 @@
         <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -616,36 +610,13 @@
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update test script auto order
</commit_message>
<xml_diff>
--- a/at_amazon/src/test/resources/data/data_order.xlsx
+++ b/at_amazon/src/test/resources/data/data_order.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t>ID TC</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Ha Noi</t>
   </si>
   <si>
-    <t>0879231543</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
@@ -91,13 +88,25 @@
   </si>
   <si>
     <t>100000</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>0823456789</t>
+  </si>
+  <si>
+    <t>'0823456789</t>
+  </si>
+  <si>
+    <t>Hmm. We couldn’t find your device’s location. Please enter the address manually.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +116,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -147,6 +163,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -455,7 +474,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -463,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,18 +517,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -518,41 +537,41 @@
         <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -564,18 +583,18 @@
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -587,18 +606,18 @@
         <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -610,13 +629,36 @@
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>